<commit_message>
No changes - fixed a weird file error
</commit_message>
<xml_diff>
--- a/demo_data.xlsx
+++ b/demo_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devon\OneDrive\Desktop\UNBC Masters\Other stuff from FFEL\Annika\PostgreSQL_demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84A902B-92FF-49EC-9823-C8CA23761ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD760CC8-2487-406F-9A14-B3A011FF485D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C574869-5971-4F48-9940-C3277AC21371}"/>
   </bookViews>
@@ -466,7 +466,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>